<commit_message>
[Admin Panel] Handle bad dates and extra columns in standards uploads better (Recidiviz/recidiviz-data#13183)
GitOrigin-RevId: 5bf1bf65125c8cb4915a8783ca72bc04c96a29fd
</commit_message>
<xml_diff>
--- a/recidiviz/tests/admin_panel/routes/fixtures/file_upload.xlsx
+++ b/recidiviz/tests/admin_panel/routes/fixtures/file_upload.xlsx
@@ -11,21 +11,234 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>string col</t>
-  </si>
-  <si>
-    <t>1 int col</t>
-  </si>
-  <si>
-    <t>_time_col</t>
-  </si>
-  <si>
-    <t>date col</t>
-  </si>
-  <si>
-    <t>bool col</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Staff ID</t>
+  </si>
+  <si>
+    <t>Staff First Name</t>
+  </si>
+  <si>
+    <t>Staff Last Name</t>
+  </si>
+  <si>
+    <t>Offender ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Address Line1</t>
+  </si>
+  <si>
+    <t>Address Line2</t>
+  </si>
+  <si>
+    <t>Address City</t>
+  </si>
+  <si>
+    <t>Address State</t>
+  </si>
+  <si>
+    <t>Address Zip</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Assignment Type</t>
+  </si>
+  <si>
+    <t>Case Type</t>
+  </si>
+  <si>
+    <t>Plan Start Date</t>
+  </si>
+  <si>
+    <t>Supervision Level</t>
+  </si>
+  <si>
+    <t>Prior Supervision Level</t>
+  </si>
+  <si>
+    <t>EXP Date</t>
+  </si>
+  <si>
+    <t>180 Day Prior EXP</t>
+  </si>
+  <si>
+    <t>Freq of FAC Contact-GT 1</t>
+  </si>
+  <si>
+    <t>FAC Note 3</t>
+  </si>
+  <si>
+    <t>FAC Note 2</t>
+  </si>
+  <si>
+    <t>FAC Note 1</t>
+  </si>
+  <si>
+    <t>FAC Note Due</t>
+  </si>
+  <si>
+    <t>Last FAC Note</t>
+  </si>
+  <si>
+    <t>Last FAC Note Type</t>
+  </si>
+  <si>
+    <t>Last FACV Date</t>
+  </si>
+  <si>
+    <t>Last FAC1 Date</t>
+  </si>
+  <si>
+    <t>Last FAC2 Date</t>
+  </si>
+  <si>
+    <t>Last HOMF Note</t>
+  </si>
+  <si>
+    <t>Last HOMF Time</t>
+  </si>
+  <si>
+    <t>Last AHOM Note</t>
+  </si>
+  <si>
+    <t>Last HOMC Note</t>
+  </si>
+  <si>
+    <t>Last HOMV Note</t>
+  </si>
+  <si>
+    <t>Last HV Type</t>
+  </si>
+  <si>
+    <t>HV Note Due</t>
+  </si>
+  <si>
+    <t>Last RIS Note</t>
+  </si>
+  <si>
+    <t>Last CCRI Note</t>
+  </si>
+  <si>
+    <t>Last CCR Date</t>
+  </si>
+  <si>
+    <t>Last Strong R</t>
+  </si>
+  <si>
+    <t>Risk Level</t>
+  </si>
+  <si>
+    <t>Alcohol/Drug Needs</t>
+  </si>
+  <si>
+    <t>Mental Health Needs</t>
+  </si>
+  <si>
+    <t>RIS Note Due</t>
+  </si>
+  <si>
+    <t>DRU Note Due</t>
+  </si>
+  <si>
+    <t>Last Sanctions Date</t>
+  </si>
+  <si>
+    <t>Last Sanctions Type</t>
+  </si>
+  <si>
+    <t>Last DRU Note</t>
+  </si>
+  <si>
+    <t>Last DRU Type</t>
+  </si>
+  <si>
+    <t>Last DRUL Note</t>
+  </si>
+  <si>
+    <t>Last EMP Note</t>
+  </si>
+  <si>
+    <t>Last EMP Type(s)</t>
+  </si>
+  <si>
+    <t>EMP Note Due</t>
+  </si>
+  <si>
+    <t>Last XEMP Date</t>
+  </si>
+  <si>
+    <t>Last EMPT Date</t>
+  </si>
+  <si>
+    <t>Last OCP Note</t>
+  </si>
+  <si>
+    <t>OCP Note Due</t>
+  </si>
+  <si>
+    <t>Last SOT Note</t>
+  </si>
+  <si>
+    <t>SOT Note Due</t>
+  </si>
+  <si>
+    <t>Last SOTT Date</t>
+  </si>
+  <si>
+    <t>Last RSS Note</t>
+  </si>
+  <si>
+    <t>Last RSS Type</t>
+  </si>
+  <si>
+    <t>RSS Note Due</t>
+  </si>
+  <si>
+    <t>Last FEE Note</t>
+  </si>
+  <si>
+    <t>FEE Note Due</t>
+  </si>
+  <si>
+    <t>Last ARR Note</t>
+  </si>
+  <si>
+    <t>Last ARR Type</t>
+  </si>
+  <si>
+    <t>ARR Note Due</t>
+  </si>
+  <si>
+    <t>Last SPE Note</t>
+  </si>
+  <si>
+    <t>SPE Note Due</t>
+  </si>
+  <si>
+    <t>Last SPET Date</t>
+  </si>
+  <si>
+    <t>Last ZZZI Date</t>
+  </si>
+  <si>
+    <t>ZZZI GT 45 days</t>
   </si>
   <si>
     <t>val a</t>
@@ -41,6 +254,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>LIFE</t>
   </si>
 </sst>
 </file>
@@ -50,15 +269,23 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,20 +302,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -305,7 +535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -323,45 +553,271 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1">
+      <c r="A2" s="2"/>
+      <c r="F2" s="2">
         <v>2.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="U2" s="3">
+        <v>44562.0</v>
+      </c>
+      <c r="AH2" s="4">
         <v>0.20555555555555555</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44562.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="2">
         <v>3.0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="AH3" s="5">
         <v>0.5242592592592593</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
+      <c r="BX3" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="2">
         <v>10.0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
+      <c r="U4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="U5" s="3">
+        <v>523456.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="U6" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>